<commit_message>
5 fix + dataset
</commit_message>
<xml_diff>
--- a/bl.xlsx
+++ b/bl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kules\Desktop\IT\Projects\Python\ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CE0159-19E2-460D-A47F-10A4FFFBD5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212954E5-BE3D-40DB-BF0F-003B48E5D542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,15 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
   <si>
-    <t>Работа</t>
-  </si>
-  <si>
-    <t>Заработок</t>
-  </si>
-  <si>
-    <t>Цель_поездки</t>
-  </si>
-  <si>
     <t>Английский_язык</t>
   </si>
   <si>
@@ -60,10 +51,19 @@
     <t>Одобрено</t>
   </si>
   <si>
-    <t>Р</t>
-  </si>
-  <si>
     <t>Средний</t>
+  </si>
+  <si>
+    <t>Претендуемая_позиция</t>
+  </si>
+  <si>
+    <t>Уровень_знаний</t>
+  </si>
+  <si>
+    <t>Опыт_разработки</t>
+  </si>
+  <si>
+    <t>И</t>
   </si>
 </sst>
 </file>
@@ -384,33 +384,33 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -418,16 +418,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -435,16 +435,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -452,16 +452,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -469,16 +469,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,16 +486,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -503,16 +503,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -520,16 +520,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -537,16 +537,16 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,16 +554,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -571,16 +571,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -588,16 +588,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -605,16 +605,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -622,16 +622,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -639,16 +639,16 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>